<commit_message>
adding new email reminder feature
</commit_message>
<xml_diff>
--- a/Sprint_Tracker.xlsx
+++ b/Sprint_Tracker.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\OneDrive\Documents\MSD_Fall_2018\book-library-web-service-hufflepuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F177C306-2031-4FDE-8394-EC8CB1236EB7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{369F2B51-C53E-4A7D-902F-FA39539755AB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6912" xr2:uid="{86C090B3-F18B-44D0-BCD0-5CB0E23A9F52}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6912" activeTab="5" xr2:uid="{86C090B3-F18B-44D0-BCD0-5CB0E23A9F52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="82">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -88,12 +92,6 @@
     <t>Design API following API Design Principles</t>
   </si>
   <si>
-    <t>Create PostgreSQL functions to be called from Flask</t>
-  </si>
-  <si>
-    <t>Implement Database models/tables in PostgreSQL</t>
-  </si>
-  <si>
     <t>Create APIs to handle basic requests and API routes in Flask</t>
   </si>
   <si>
@@ -131,6 +129,153 @@
   </si>
   <si>
     <t>Deploy Basic APIs with Postgres and Flask application to heroku</t>
+  </si>
+  <si>
+    <t>Create demo PostgreSQL functions to be called from Flask</t>
+  </si>
+  <si>
+    <t>Create a Middleware layer that connects database layer to routes module</t>
+  </si>
+  <si>
+    <t>Set up the project structure - divide the project into layers</t>
+  </si>
+  <si>
+    <t>Connect GitHub repository to Heroku</t>
+  </si>
+  <si>
+    <t>Configure CI/CD on Heroku for automatic deployments</t>
+  </si>
+  <si>
+    <t>Create a development pipeline on Heroku for Hufflepuff repository</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Continuous deployment by pushing to master branch.  </t>
+  </si>
+  <si>
+    <t>Configure one or more routes and handle them in separate modules</t>
+  </si>
+  <si>
+    <t>Implement Database models in python classes</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Oct 03 - Oct 9</t>
+  </si>
+  <si>
+    <t>Implement Flask-restplus for swagger API design documentation</t>
+  </si>
+  <si>
+    <t>Check Swagger API design documentation</t>
+  </si>
+  <si>
+    <t>Research for plug-ins for creating swagger API Documentation</t>
+  </si>
+  <si>
+    <t>Check and Install Flask Restplus library</t>
+  </si>
+  <si>
+    <t>Implement annotations for existing APIs</t>
+  </si>
+  <si>
+    <t>Change APIs and establish new routes using Flask-restplus</t>
+  </si>
+  <si>
+    <t>Establish response types to all APIs</t>
+  </si>
+  <si>
+    <t>Create Middleware methods as helper functions to API routes</t>
+  </si>
+  <si>
+    <t>Re-design Database models to support required API functionality</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>5,6,7</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Oct 10 - Oct 16</t>
+  </si>
+  <si>
+    <t>Implement Data persistance</t>
+  </si>
+  <si>
+    <t>Check libraries for adding data persistance to Flask Application</t>
+  </si>
+  <si>
+    <t>Research sqlalchemy and install flask-sqlalchemy</t>
+  </si>
+  <si>
+    <t>setup connection to Heroku PostgreSQL server</t>
+  </si>
+  <si>
+    <t>setup and implement a demo application to use PostgreSQL server</t>
+  </si>
+  <si>
+    <t>Create database connection and session and incorporate to app</t>
+  </si>
+  <si>
+    <t>Implement CRUD applications on basic resources</t>
+  </si>
+  <si>
+    <t>Create and test tables in PostgreSQL server</t>
+  </si>
+  <si>
+    <t>Test the resources and some routes and check data persistance</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Oct 17 - Oct 23</t>
+  </si>
+  <si>
+    <t>Follow API Design Guidelines</t>
+  </si>
+  <si>
+    <t>Check API design principles and review them</t>
+  </si>
+  <si>
+    <t>Re-design the API following Design Principles</t>
+  </si>
+  <si>
+    <t>Establish response types and statuses for all the API routes</t>
+  </si>
+  <si>
+    <t>Test API design and response types for all the API routes</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Oct 24 - Oct 30</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
+  </si>
+  <si>
+    <t>Conduct code review</t>
+  </si>
+  <si>
+    <t>Create new branches to implement new features</t>
+  </si>
+  <si>
+    <t>Complete working on these features</t>
+  </si>
+  <si>
+    <t>create different pull requests for these features</t>
+  </si>
+  <si>
+    <t>review and merge the code to the master branch</t>
+  </si>
+  <si>
+    <t>Code Reviews</t>
   </si>
 </sst>
 </file>
@@ -503,10 +648,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F351B-3A22-4A34-BEE3-6C12013A6A6A}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,10 +726,10 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -599,7 +747,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -705,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -734,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -758,7 +906,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -770,7 +918,7 @@
         <v>0.5</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -787,10 +935,10 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
@@ -802,12 +950,12 @@
         <v>9</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16">
         <f xml:space="preserve"> SUM(G5:G13)</f>
@@ -816,7 +964,7 @@
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -824,7 +972,7 @@
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -832,12 +980,12 @@
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +996,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86A4FB16-F5A0-4BCB-98B2-97A0AB1DFE2C}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,12 +1010,12 @@
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -874,10 +1025,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
@@ -914,133 +1065,257 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
       <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
       <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
       <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
       <c r="H9" s="3"/>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>9</v>
       </c>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14">
-        <v>10</v>
-      </c>
-      <c r="H14" s="3"/>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -1048,7 +1323,7 @@
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -1056,12 +1331,1204 @@
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9148C7CF-B274-4BAF-A0CE-2CE0AE65560D}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17EB690-886F-452A-8482-EC09B6658FBF}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B61CF0-D079-4A0F-BF4C-C862EE085168}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="A1:I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2637D2E9-3160-4660-B0B8-EBF05EF1160D}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>